<commit_message>
I FUCKING DID IT HOLY SHIT
</commit_message>
<xml_diff>
--- a/ncx.xlsx
+++ b/ncx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,363 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>253e459e0dc3de445fa4eea651a139ce</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>&amp; &amp; Nona</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>9d473a7444ef6f4d080d54aec4891d54</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Balinca &amp; Malaviya</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Balinca &amp; Malaviya</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>f35ef701dc13b011bec2afcf484c8012</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>&amp; &amp; Nona</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Jain &amp; Soto</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>84f2719afb36ce7fdbc3beb60db757e2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Balinca &amp; Malaviya</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Balinca &amp; Malaviya</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>f7e13e407a5118847f496248141430dc</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Balinca &amp; Malaviya</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>&amp; &amp; Nona</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>04836fee5898f9fdabbd670dd2653d6f</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>de2cc1e82c2afc223353af87dde50120</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>c2af907400143736d98450762d476166</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Jonas &amp; Shah</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>7b2e92147ae6b6df75feff482e8cd5b6</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Jain &amp; Soto</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Jain &amp; Soto</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04a58f03b18e2a5bd95f07b690d1e41d</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Jain &amp; Soto</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Jain &amp; Soto</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04a31d23d25ac871a736c56c72019452</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Balinca &amp; Malaviya</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jonas &amp; Shah</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>59de1679647fb75c8fafbfe0f4de61c8</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Jain &amp; Soto</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Jonas &amp; Shah</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>b0c7cbbcfa39294c5921ae5efc085d5c</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2882092cedd64231c4ed11d4cb5e4d97</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Zhao &amp; jagtap</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>91613214ec3950a0599d5a096dc32aa6</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Lin &amp; Nguyen</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Diehl &amp; Dowler</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>e4845b639f3f3d68c9cb38a989fb12da</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Lin &amp; Nguyen</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>b5f9449672616417b46e61686d22006c</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Diehl &amp; Dowler</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Kim &amp; Sumesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>546524b567831e12f2a3054e080c6f85</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Lin &amp; Nguyen</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Kim &amp; Sumesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>273f10b7459e5be69a257b8acd7a36f0</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Zhao &amp; jagtap</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Diehl &amp; Dowler</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>70dac1be21ceb1ddfba60064a770a883</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Kim &amp; Sumesh</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Zhao &amp; jagtap</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>91b4647cf403ae6f3fc4b0b087947417</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Mohapatra &amp; Verma</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Diehl &amp; Dowler</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>